<commit_message>
Update deep dive word counts
</commit_message>
<xml_diff>
--- a/code-analysis/word-count-deep-dives/Deep-dives-word-counts.xlsx
+++ b/code-analysis/word-count-deep-dives/Deep-dives-word-counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10112"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mark/Documents/Files/Websites/Repositories/bbcelite-scripts/code-analysis/word-count-deep-dives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{608C9015-EB2A-8F47-8149-34CAA85FEDDD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08579EE1-7F07-F945-9D5A-6A9220BFC7C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1400" yWindow="1720" windowWidth="19940" windowHeight="17440" xr2:uid="{B861FA09-B3AD-9448-956B-DECF27F030C1}"/>
+    <workbookView xWindow="15540" yWindow="2540" windowWidth="19940" windowHeight="17440" xr2:uid="{B861FA09-B3AD-9448-956B-DECF27F030C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="236">
   <si>
     <t>Elite</t>
   </si>
@@ -702,6 +702,48 @@
   </si>
   <si>
     <t>lander.bbcelite.com/deep_dives/index.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/a_sense_of_scale.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/comparing_ship_specifications.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/docked_and_flight_code.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/colouring_the_commodore_64_bitmap_screen.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/music_in_commodore_64_elite.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/building_commodore_64_elite_from_the_source_disk.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/the_split-screen_mode_commodore_64.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/the_elite_memory_map_commodore_64.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/developing_commodore_64_elite_on_a_bbc_micro.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/reading_the_commodore_64_keyboard_matrix.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/drawing_pixels_in_the_commodore_64_version.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/sound_effects_in_commodore_64_elite.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/the_elite_memory_map_apple_ii.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/sprite_usage_in_commodore_64_elite.html</t>
   </si>
 </sst>
 </file>
@@ -1078,9 +1120,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE93E83-D4E6-9644-A232-80EA76D69371}">
   <dimension ref="A1:C9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C7" sqref="C7"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1102,11 +1142,11 @@
       </c>
       <c r="B2" s="4">
         <f>SUMIF(wordcount.txt!B:B,"*elite.bbcelite.com*",wordcount.txt!A:A)</f>
-        <v>170082</v>
+        <v>199158</v>
       </c>
       <c r="C2" s="6">
         <f>B2/$B$7</f>
-        <v>0.455613804335888</v>
+        <v>0.49495619757688725</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1119,7 +1159,7 @@
       </c>
       <c r="C3" s="6">
         <f>B3/$B$7</f>
-        <v>0.33691398140384621</v>
+        <v>0.31257160608884749</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1128,11 +1168,11 @@
       </c>
       <c r="B4" s="4">
         <f>SUMIF(wordcount.txt!B:B,"*aviator.bbcelite.com*",wordcount.txt!A:A)</f>
-        <v>41268</v>
+        <v>41264</v>
       </c>
       <c r="C4" s="6">
         <f>B4/$B$7</f>
-        <v>0.11054826776104131</v>
+        <v>0.10255110282696489</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -1145,7 +1185,7 @@
       </c>
       <c r="C5" s="6">
         <f>B5/$B$7</f>
-        <v>9.6923946499224492E-2</v>
+        <v>8.9921093507300404E-2</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
@@ -1157,7 +1197,7 @@
       </c>
       <c r="B7" s="5">
         <f>SUM(B2:B5)</f>
-        <v>373303</v>
+        <v>402375</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1173,9 +1213,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB40F6A-245F-024F-9684-E7DD745D31B2}">
-  <dimension ref="A1:B214"/>
+  <dimension ref="A1:B228"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B229"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1201,1697 +1243,1809 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A3" s="1">
-        <v>4163</v>
+        <v>5185</v>
       </c>
       <c r="B3" t="s">
-        <v>10</v>
+        <v>222</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>3182</v>
+        <v>4163</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>3087</v>
+        <v>3402</v>
       </c>
       <c r="B5" t="s">
-        <v>12</v>
+        <v>223</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
-        <v>2925</v>
+        <v>3182</v>
       </c>
       <c r="B6" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>2783</v>
+        <v>3087</v>
       </c>
       <c r="B7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>2772</v>
+        <v>2995</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
-        <v>2705</v>
+        <v>2844</v>
       </c>
       <c r="B9" t="s">
-        <v>16</v>
+        <v>224</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
-        <v>2666</v>
+        <v>2826</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A11" s="1">
-        <v>2601</v>
+        <v>2783</v>
       </c>
       <c r="B11" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A12" s="1">
-        <v>2456</v>
+        <v>2707</v>
       </c>
       <c r="B12" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>2399</v>
+        <v>2666</v>
       </c>
       <c r="B13" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>2398</v>
+        <v>2650</v>
       </c>
       <c r="B14" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>2369</v>
+        <v>2569</v>
       </c>
       <c r="B15" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>2321</v>
+        <v>2542</v>
       </c>
       <c r="B16" t="s">
-        <v>23</v>
+        <v>225</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>2313</v>
+        <v>2525</v>
       </c>
       <c r="B17" t="s">
-        <v>24</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>2308</v>
+        <v>2456</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>2283</v>
+        <v>2398</v>
       </c>
       <c r="B19" t="s">
-        <v>26</v>
+        <v>21</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="1">
-        <v>2215</v>
+        <v>2371</v>
       </c>
       <c r="B20" t="s">
-        <v>27</v>
+        <v>22</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>2205</v>
+        <v>2321</v>
       </c>
       <c r="B21" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="1">
-        <v>2198</v>
+        <v>2314</v>
       </c>
       <c r="B22" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="1">
-        <v>2191</v>
+        <v>2308</v>
       </c>
       <c r="B23" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>2127</v>
+        <v>2283</v>
       </c>
       <c r="B24" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>2035</v>
+        <v>2221</v>
       </c>
       <c r="B25" t="s">
-        <v>32</v>
+        <v>27</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>1918</v>
+        <v>2219</v>
       </c>
       <c r="B26" t="s">
-        <v>33</v>
+        <v>28</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>1916</v>
+        <v>2141</v>
       </c>
       <c r="B27" t="s">
-        <v>34</v>
+        <v>226</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>1913</v>
+        <v>2131</v>
       </c>
       <c r="B28" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>1897</v>
+        <v>2035</v>
       </c>
       <c r="B29" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>1870</v>
+        <v>2034</v>
       </c>
       <c r="B30" t="s">
-        <v>37</v>
+        <v>227</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>1857</v>
+        <v>1961</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>1829</v>
+        <v>1955</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>228</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>1821</v>
+        <v>1918</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>33</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>1795</v>
+        <v>1913</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>35</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>1758</v>
+        <v>1887</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>36</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>1721</v>
+        <v>1870</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>1714</v>
+        <v>1857</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>1686</v>
+        <v>1834</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>1669</v>
+        <v>1829</v>
       </c>
       <c r="B39" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>1660</v>
+        <v>1796</v>
       </c>
       <c r="B40" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>1600</v>
+        <v>1795</v>
       </c>
       <c r="B41" t="s">
-        <v>48</v>
+        <v>41</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>1593</v>
+        <v>1759</v>
       </c>
       <c r="B42" t="s">
-        <v>49</v>
+        <v>46</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>1582</v>
+        <v>1758</v>
       </c>
       <c r="B43" t="s">
-        <v>50</v>
+        <v>42</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>1570</v>
+        <v>1721</v>
       </c>
       <c r="B44" t="s">
-        <v>51</v>
+        <v>43</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>1570</v>
+        <v>1714</v>
       </c>
       <c r="B45" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>1560</v>
+        <v>1713</v>
       </c>
       <c r="B46" t="s">
-        <v>53</v>
+        <v>229</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>1559</v>
+        <v>1690</v>
       </c>
       <c r="B47" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>1555</v>
+        <v>1660</v>
       </c>
       <c r="B48" t="s">
-        <v>55</v>
+        <v>47</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>1540</v>
+        <v>1621</v>
       </c>
       <c r="B49" t="s">
-        <v>56</v>
+        <v>52</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>1513</v>
+        <v>1600</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>1506</v>
+        <v>1593</v>
       </c>
       <c r="B51" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>1473</v>
+        <v>1587</v>
       </c>
       <c r="B52" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>1453</v>
+        <v>1580</v>
       </c>
       <c r="B53" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>1450</v>
+        <v>1570</v>
       </c>
       <c r="B54" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>1414</v>
+        <v>1565</v>
       </c>
       <c r="B55" t="s">
-        <v>62</v>
+        <v>54</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>1409</v>
+        <v>1560</v>
       </c>
       <c r="B56" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>1371</v>
+        <v>1560</v>
       </c>
       <c r="B57" t="s">
-        <v>64</v>
+        <v>53</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>1362</v>
+        <v>1553</v>
       </c>
       <c r="B58" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>1345</v>
+        <v>1513</v>
       </c>
       <c r="B59" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>1333</v>
+        <v>1506</v>
       </c>
       <c r="B60" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>1314</v>
+        <v>1475</v>
       </c>
       <c r="B61" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>1292</v>
+        <v>1453</v>
       </c>
       <c r="B62" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>1282</v>
+        <v>1450</v>
       </c>
       <c r="B63" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>1244</v>
+        <v>1433</v>
       </c>
       <c r="B64" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
-        <v>1237</v>
+        <v>1409</v>
       </c>
       <c r="B65" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>1217</v>
+        <v>1390</v>
       </c>
       <c r="B66" t="s">
-        <v>73</v>
+        <v>65</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>1200</v>
+        <v>1388</v>
       </c>
       <c r="B67" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>1169</v>
+        <v>1354</v>
       </c>
       <c r="B68" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>1127</v>
+        <v>1351</v>
       </c>
       <c r="B69" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>1104</v>
+        <v>1310</v>
       </c>
       <c r="B70" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>1076</v>
+        <v>1295</v>
       </c>
       <c r="B71" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>1040</v>
+        <v>1290</v>
       </c>
       <c r="B72" t="s">
-        <v>79</v>
+        <v>69</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>1036</v>
+        <v>1282</v>
       </c>
       <c r="B73" t="s">
-        <v>80</v>
+        <v>70</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>1034</v>
+        <v>1263</v>
       </c>
       <c r="B74" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>1032</v>
+        <v>1238</v>
       </c>
       <c r="B75" t="s">
-        <v>82</v>
+        <v>72</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
-        <v>1027</v>
+        <v>1221</v>
       </c>
       <c r="B76" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>1020</v>
+        <v>1169</v>
       </c>
       <c r="B77" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
-        <v>1007</v>
+        <v>1134</v>
       </c>
       <c r="B78" t="s">
-        <v>85</v>
+        <v>230</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>950</v>
+        <v>1127</v>
       </c>
       <c r="B79" t="s">
-        <v>86</v>
+        <v>231</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>933</v>
+        <v>1125</v>
       </c>
       <c r="B80" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>925</v>
+        <v>1114</v>
       </c>
       <c r="B81" t="s">
-        <v>88</v>
+        <v>232</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>914</v>
+        <v>1104</v>
       </c>
       <c r="B82" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>873</v>
+        <v>1083</v>
       </c>
       <c r="B83" t="s">
-        <v>90</v>
+        <v>73</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>869</v>
+        <v>1076</v>
       </c>
       <c r="B84" t="s">
-        <v>91</v>
+        <v>78</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
-        <v>853</v>
+        <v>1073</v>
       </c>
       <c r="B85" t="s">
-        <v>92</v>
+        <v>81</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>838</v>
+        <v>1032</v>
       </c>
       <c r="B86" t="s">
-        <v>93</v>
+        <v>82</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>817</v>
+        <v>1027</v>
       </c>
       <c r="B87" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>808</v>
+        <v>1027</v>
       </c>
       <c r="B88" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>806</v>
+        <v>1023</v>
       </c>
       <c r="B89" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>787</v>
+        <v>1018</v>
       </c>
       <c r="B90" t="s">
-        <v>97</v>
+        <v>233</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>771</v>
+        <v>1006</v>
       </c>
       <c r="B91" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>769</v>
+        <v>950</v>
       </c>
       <c r="B92" t="s">
-        <v>99</v>
+        <v>86</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
-        <v>744</v>
+        <v>933</v>
       </c>
       <c r="B93" t="s">
-        <v>100</v>
+        <v>87</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>735</v>
+        <v>928</v>
       </c>
       <c r="B94" t="s">
-        <v>101</v>
+        <v>88</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
-        <v>711</v>
+        <v>914</v>
       </c>
       <c r="B95" t="s">
-        <v>102</v>
+        <v>89</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>663</v>
+        <v>903</v>
       </c>
       <c r="B96" t="s">
-        <v>103</v>
+        <v>97</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
-        <v>658</v>
+        <v>873</v>
       </c>
       <c r="B97" t="s">
-        <v>104</v>
+        <v>90</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A98" s="1">
-        <v>590</v>
+        <v>869</v>
       </c>
       <c r="B98" t="s">
-        <v>105</v>
+        <v>91</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
-        <v>559</v>
+        <v>838</v>
       </c>
       <c r="B99" t="s">
-        <v>106</v>
+        <v>93</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>557</v>
+        <v>817</v>
       </c>
       <c r="B100" t="s">
-        <v>107</v>
+        <v>94</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>535</v>
+        <v>808</v>
       </c>
       <c r="B101" t="s">
-        <v>108</v>
+        <v>95</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>501</v>
+        <v>806</v>
       </c>
       <c r="B102" t="s">
-        <v>109</v>
+        <v>96</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>487</v>
+        <v>804</v>
       </c>
       <c r="B103" t="s">
-        <v>110</v>
+        <v>99</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>486</v>
+        <v>771</v>
       </c>
       <c r="B104" t="s">
-        <v>111</v>
+        <v>98</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>476</v>
+        <v>746</v>
       </c>
       <c r="B105" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>355</v>
+        <v>737</v>
       </c>
       <c r="B106" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>353</v>
+        <v>730</v>
       </c>
       <c r="B107" t="s">
-        <v>114</v>
+        <v>104</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>339</v>
+        <v>713</v>
       </c>
       <c r="B108" t="s">
-        <v>115</v>
+        <v>102</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>286</v>
+        <v>663</v>
       </c>
       <c r="B109" t="s">
-        <v>116</v>
+        <v>103</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>273</v>
+        <v>590</v>
       </c>
       <c r="B110" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <v>7326</v>
+        <v>560</v>
       </c>
       <c r="B111" t="s">
-        <v>118</v>
+        <v>234</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
-        <v>5383</v>
+        <v>559</v>
       </c>
       <c r="B112" t="s">
-        <v>119</v>
+        <v>106</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>5182</v>
+        <v>557</v>
       </c>
       <c r="B113" t="s">
-        <v>120</v>
+        <v>107</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>4858</v>
+        <v>556</v>
       </c>
       <c r="B114" t="s">
-        <v>121</v>
+        <v>235</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <v>4837</v>
+        <v>535</v>
       </c>
       <c r="B115" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <v>4702</v>
+        <v>488</v>
       </c>
       <c r="B116" t="s">
-        <v>123</v>
+        <v>109</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <v>4682</v>
+        <v>487</v>
       </c>
       <c r="B117" t="s">
-        <v>124</v>
+        <v>110</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <v>4004</v>
+        <v>486</v>
       </c>
       <c r="B118" t="s">
-        <v>125</v>
+        <v>111</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <v>3775</v>
+        <v>476</v>
       </c>
       <c r="B119" t="s">
-        <v>126</v>
+        <v>112</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>3688</v>
+        <v>355</v>
       </c>
       <c r="B120" t="s">
-        <v>127</v>
+        <v>113</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <v>3646</v>
+        <v>353</v>
       </c>
       <c r="B121" t="s">
-        <v>128</v>
+        <v>114</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
-        <v>3640</v>
+        <v>339</v>
       </c>
       <c r="B122" t="s">
-        <v>129</v>
+        <v>115</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
-        <v>3293</v>
+        <v>286</v>
       </c>
       <c r="B123" t="s">
-        <v>130</v>
+        <v>116</v>
       </c>
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>3267</v>
+        <v>273</v>
       </c>
       <c r="B124" t="s">
-        <v>131</v>
+        <v>117</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
-        <v>3208</v>
+        <v>7326</v>
       </c>
       <c r="B125" t="s">
-        <v>132</v>
+        <v>118</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
-        <v>3178</v>
+        <v>5383</v>
       </c>
       <c r="B126" t="s">
-        <v>133</v>
+        <v>119</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
-        <v>3156</v>
+        <v>5182</v>
       </c>
       <c r="B127" t="s">
-        <v>134</v>
+        <v>120</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
-        <v>3074</v>
+        <v>4858</v>
       </c>
       <c r="B128" t="s">
-        <v>135</v>
+        <v>121</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
-        <v>3007</v>
+        <v>4837</v>
       </c>
       <c r="B129" t="s">
-        <v>136</v>
+        <v>122</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
-        <v>2923</v>
+        <v>4702</v>
       </c>
       <c r="B130" t="s">
-        <v>137</v>
+        <v>123</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
-        <v>2857</v>
+        <v>4682</v>
       </c>
       <c r="B131" t="s">
-        <v>138</v>
+        <v>124</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
-        <v>2852</v>
+        <v>4004</v>
       </c>
       <c r="B132" t="s">
-        <v>139</v>
+        <v>125</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
-        <v>2550</v>
+        <v>3775</v>
       </c>
       <c r="B133" t="s">
-        <v>140</v>
+        <v>126</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>2524</v>
+        <v>3688</v>
       </c>
       <c r="B134" t="s">
-        <v>141</v>
+        <v>127</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
-        <v>2489</v>
+        <v>3646</v>
       </c>
       <c r="B135" t="s">
-        <v>142</v>
+        <v>128</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
-        <v>2188</v>
+        <v>3640</v>
       </c>
       <c r="B136" t="s">
-        <v>143</v>
+        <v>129</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
-        <v>2080</v>
+        <v>3293</v>
       </c>
       <c r="B137" t="s">
-        <v>144</v>
+        <v>130</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
-        <v>1966</v>
+        <v>3267</v>
       </c>
       <c r="B138" t="s">
-        <v>145</v>
+        <v>131</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
-        <v>1890</v>
+        <v>3208</v>
       </c>
       <c r="B139" t="s">
-        <v>146</v>
+        <v>132</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
-        <v>1878</v>
+        <v>3178</v>
       </c>
       <c r="B140" t="s">
-        <v>147</v>
+        <v>133</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
-        <v>1675</v>
+        <v>3156</v>
       </c>
       <c r="B141" t="s">
-        <v>148</v>
+        <v>134</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
-        <v>1585</v>
+        <v>3074</v>
       </c>
       <c r="B142" t="s">
-        <v>149</v>
+        <v>135</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
-        <v>1582</v>
+        <v>3007</v>
       </c>
       <c r="B143" t="s">
-        <v>150</v>
+        <v>136</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>1427</v>
+        <v>2923</v>
       </c>
       <c r="B144" t="s">
-        <v>151</v>
+        <v>137</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>1405</v>
+        <v>2857</v>
       </c>
       <c r="B145" t="s">
-        <v>152</v>
+        <v>138</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>1320</v>
+        <v>2852</v>
       </c>
       <c r="B146" t="s">
-        <v>153</v>
+        <v>139</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>1283</v>
+        <v>2550</v>
       </c>
       <c r="B147" t="s">
-        <v>154</v>
+        <v>140</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>1148</v>
+        <v>2524</v>
       </c>
       <c r="B148" t="s">
-        <v>155</v>
+        <v>141</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>1122</v>
+        <v>2489</v>
       </c>
       <c r="B149" t="s">
-        <v>156</v>
+        <v>142</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
-        <v>1065</v>
+        <v>2188</v>
       </c>
       <c r="B150" t="s">
-        <v>157</v>
+        <v>143</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
-        <v>1040</v>
+        <v>2080</v>
       </c>
       <c r="B151" t="s">
-        <v>158</v>
+        <v>144</v>
       </c>
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
-        <v>1010</v>
+        <v>1966</v>
       </c>
       <c r="B152" t="s">
-        <v>159</v>
+        <v>145</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
-        <v>1004</v>
+        <v>1890</v>
       </c>
       <c r="B153" t="s">
-        <v>160</v>
+        <v>146</v>
       </c>
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
-        <v>973</v>
+        <v>1878</v>
       </c>
       <c r="B154" t="s">
-        <v>161</v>
+        <v>147</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
-        <v>888</v>
+        <v>1675</v>
       </c>
       <c r="B155" t="s">
-        <v>162</v>
+        <v>148</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
-        <v>842</v>
+        <v>1585</v>
       </c>
       <c r="B156" t="s">
-        <v>163</v>
+        <v>149</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
-        <v>735</v>
+        <v>1582</v>
       </c>
       <c r="B157" t="s">
-        <v>164</v>
+        <v>150</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>717</v>
+        <v>1427</v>
       </c>
       <c r="B158" t="s">
-        <v>165</v>
+        <v>151</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>562</v>
+        <v>1405</v>
       </c>
       <c r="B159" t="s">
-        <v>166</v>
+        <v>152</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
-        <v>285</v>
+        <v>1320</v>
       </c>
       <c r="B160" t="s">
-        <v>167</v>
+        <v>153</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
-        <v>3627</v>
+        <v>1283</v>
       </c>
       <c r="B161" t="s">
-        <v>168</v>
+        <v>154</v>
       </c>
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>2508</v>
+        <v>1148</v>
       </c>
       <c r="B162" t="s">
-        <v>169</v>
+        <v>155</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>2367</v>
+        <v>1122</v>
       </c>
       <c r="B163" t="s">
-        <v>170</v>
+        <v>156</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>2117</v>
+        <v>1065</v>
       </c>
       <c r="B164" t="s">
-        <v>171</v>
+        <v>157</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>2027</v>
+        <v>1040</v>
       </c>
       <c r="B165" t="s">
-        <v>172</v>
+        <v>158</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>1587</v>
+        <v>1010</v>
       </c>
       <c r="B166" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>1532</v>
+        <v>1004</v>
       </c>
       <c r="B167" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>1369</v>
+        <v>973</v>
       </c>
       <c r="B168" t="s">
-        <v>175</v>
+        <v>161</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>1368</v>
+        <v>888</v>
       </c>
       <c r="B169" t="s">
-        <v>176</v>
+        <v>162</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>1349</v>
+        <v>842</v>
       </c>
       <c r="B170" t="s">
-        <v>177</v>
+        <v>163</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
-        <v>1336</v>
+        <v>735</v>
       </c>
       <c r="B171" t="s">
-        <v>178</v>
+        <v>164</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
-        <v>1312</v>
+        <v>717</v>
       </c>
       <c r="B172" t="s">
-        <v>179</v>
+        <v>165</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
-        <v>1299</v>
+        <v>562</v>
       </c>
       <c r="B173" t="s">
-        <v>180</v>
+        <v>166</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
-        <v>1267</v>
+        <v>285</v>
       </c>
       <c r="B174" t="s">
-        <v>181</v>
+        <v>167</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
-        <v>1260</v>
+        <v>3627</v>
       </c>
       <c r="B175" t="s">
-        <v>182</v>
+        <v>168</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
-        <v>1258</v>
+        <v>2508</v>
       </c>
       <c r="B176" t="s">
-        <v>183</v>
+        <v>169</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>1147</v>
+        <v>2367</v>
       </c>
       <c r="B177" t="s">
-        <v>184</v>
+        <v>170</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
-        <v>1147</v>
+        <v>2117</v>
       </c>
       <c r="B178" t="s">
-        <v>185</v>
+        <v>171</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>1145</v>
+        <v>2027</v>
       </c>
       <c r="B179" t="s">
-        <v>186</v>
+        <v>172</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
-        <v>1139</v>
+        <v>1587</v>
       </c>
       <c r="B180" t="s">
-        <v>187</v>
+        <v>173</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
-        <v>1074</v>
+        <v>1532</v>
       </c>
       <c r="B181" t="s">
-        <v>188</v>
+        <v>174</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>1025</v>
+        <v>1369</v>
       </c>
       <c r="B182" t="s">
-        <v>189</v>
+        <v>175</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>914</v>
+        <v>1368</v>
       </c>
       <c r="B183" t="s">
-        <v>190</v>
+        <v>176</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
-        <v>892</v>
+        <v>1349</v>
       </c>
       <c r="B184" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
-        <v>887</v>
+        <v>1336</v>
       </c>
       <c r="B185" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
-        <v>749</v>
+        <v>1312</v>
       </c>
       <c r="B186" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>676</v>
+        <v>1299</v>
       </c>
       <c r="B187" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
-        <v>673</v>
+        <v>1267</v>
       </c>
       <c r="B188" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
-        <v>641</v>
+        <v>1260</v>
       </c>
       <c r="B189" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
-        <v>613</v>
+        <v>1258</v>
       </c>
       <c r="B190" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
-        <v>593</v>
+        <v>1147</v>
       </c>
       <c r="B191" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
-        <v>370</v>
+        <v>1147</v>
       </c>
       <c r="B192" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
-        <v>3252</v>
+        <v>1145</v>
       </c>
       <c r="B193" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
-        <v>3028</v>
+        <v>1139</v>
       </c>
       <c r="B194" t="s">
-        <v>201</v>
+        <v>187</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
-        <v>3015</v>
+        <v>1074</v>
       </c>
       <c r="B195" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
-        <v>2939</v>
+        <v>1025</v>
       </c>
       <c r="B196" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
-        <v>2793</v>
+        <v>910</v>
       </c>
       <c r="B197" t="s">
-        <v>204</v>
+        <v>190</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
-        <v>2613</v>
+        <v>892</v>
       </c>
       <c r="B198" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
-        <v>2602</v>
+        <v>887</v>
       </c>
       <c r="B199" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
-        <v>2170</v>
+        <v>749</v>
       </c>
       <c r="B200" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
-        <v>1924</v>
+        <v>676</v>
       </c>
       <c r="B201" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
-        <v>1517</v>
+        <v>673</v>
       </c>
       <c r="B202" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
-        <v>1424</v>
+        <v>641</v>
       </c>
       <c r="B203" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
-        <v>1384</v>
+        <v>613</v>
       </c>
       <c r="B204" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
-        <v>1225</v>
+        <v>593</v>
       </c>
       <c r="B205" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
-        <v>1037</v>
+        <v>370</v>
       </c>
       <c r="B206" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
-        <v>874</v>
+        <v>3252</v>
       </c>
       <c r="B207" t="s">
-        <v>214</v>
+        <v>200</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
-        <v>851</v>
+        <v>3028</v>
       </c>
       <c r="B208" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
-        <v>799</v>
+        <v>3015</v>
       </c>
       <c r="B209" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
-        <v>667</v>
+        <v>2939</v>
       </c>
       <c r="B210" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
-        <v>665</v>
+        <v>2793</v>
       </c>
       <c r="B211" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
-        <v>483</v>
+        <v>2613</v>
       </c>
       <c r="B212" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
-        <v>468</v>
+        <v>2602</v>
       </c>
       <c r="B213" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
+        <v>2170</v>
+      </c>
+      <c r="B214" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="215" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A215" s="1">
+        <v>1924</v>
+      </c>
+      <c r="B215" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="216" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A216" s="1">
+        <v>1517</v>
+      </c>
+      <c r="B216" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="217" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A217" s="1">
+        <v>1424</v>
+      </c>
+      <c r="B217" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="218" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A218" s="1">
+        <v>1384</v>
+      </c>
+      <c r="B218" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="219" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A219" s="1">
+        <v>1225</v>
+      </c>
+      <c r="B219" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="220" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A220" s="1">
+        <v>1037</v>
+      </c>
+      <c r="B220" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="221" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A221" s="1">
+        <v>874</v>
+      </c>
+      <c r="B221" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="222" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A222" s="1">
+        <v>851</v>
+      </c>
+      <c r="B222" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="223" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A223" s="1">
+        <v>799</v>
+      </c>
+      <c r="B223" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="224" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A224" s="1">
+        <v>667</v>
+      </c>
+      <c r="B224" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="225" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A225" s="1">
+        <v>665</v>
+      </c>
+      <c r="B225" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="226" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A226" s="1">
+        <v>483</v>
+      </c>
+      <c r="B226" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="227" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A227" s="1">
+        <v>468</v>
+      </c>
+      <c r="B227" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="228" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A228" s="1">
         <v>452</v>
       </c>
-      <c r="B214" t="s">
+      <c r="B228" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Add The Sentinel to deep dive word count
</commit_message>
<xml_diff>
--- a/code-analysis/word-count-deep-dives/Deep-dives-word-counts.xlsx
+++ b/code-analysis/word-count-deep-dives/Deep-dives-word-counts.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10215"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Mark/Documents/Files/Websites/Repositories/bbcelite-scripts/code-analysis/word-count-deep-dives/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2D0357EE-8E7E-0B40-A86D-48A01F06DADE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1189DB4-C3F9-1A45-82FD-D124F85DC0DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15540" yWindow="2540" windowWidth="19940" windowHeight="17440" activeTab="1" xr2:uid="{B861FA09-B3AD-9448-956B-DECF27F030C1}"/>
+    <workbookView xWindow="15540" yWindow="2540" windowWidth="19940" windowHeight="17440" xr2:uid="{B861FA09-B3AD-9448-956B-DECF27F030C1}"/>
   </bookViews>
   <sheets>
     <sheet name="Results" sheetId="3" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="243" uniqueCount="243">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="296" uniqueCount="296">
   <si>
     <t>Elite</t>
   </si>
@@ -765,6 +765,165 @@
   </si>
   <si>
     <t>elite.bbcelite.com/deep_dives/working_with_the_apple_ii_keyboard.html</t>
+  </si>
+  <si>
+    <t>elite.bbcelite.com/deep_dives/aggression_and_hostility_in_ship_tactics.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/generating_the_landscape.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/adding_enemies_and_trees_to_the_landscape.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/trigonometry_in_8-bit_assembly.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/program_flow_of_the_gameplay_loop.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/cartesian_coordinates.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/program_flow_of_the_main_title_loop.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/tile_data.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/program_flow_of_the_main_game_loop.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/tile_shapes.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/the_sentinel_memory_map.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/the_projection_system.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/seed_number_generation.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/screen_buffers.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/index.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/the_interrupt_handler.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/calculating_the_hypotenuse.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/pitch_and_yaw_angles.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/converting_angles_to_coordinates.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/reusing_the_geometry_routines_from_revs.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/converting_coordinates_to_angles.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/entry_and_setup_code.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/the_landscape_secret_code.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/music.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/text_tokens.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/drawing_the_title_screens.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/the_custom_screen_mode.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/object_spawning.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/panning_and_hardware_scrolling.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/drawing_the_landscape_view.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/dithering_to_the_screen.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/3d_object_definitions.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/the_visibility_table.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/drawing_the_landscape_preview.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/3d_text_using_blocks.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/the_drawing_tables.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/calculating_angles_for_the_landscape_view.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/anti-cracker_checks.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/drawing_objects.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/stacking_objects.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/the_energy_icons.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/enemy_tactics.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/random_number_generation.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/calculating_gaze.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/the_scanner.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/the_key_logger.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/game_timings.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/drawing_filled_polygons.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/colours_and_palettes.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/the_crosshair_sights.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/sound_effects.html</t>
+  </si>
+  <si>
+    <t>/Users/Mark/Sites/bbcelite-websites/thesentinel.bbcelite.com/deep_dives/source_code_clues_hidden_in_the_game_binary.html</t>
+  </si>
+  <si>
+    <t>The Sentinel</t>
   </si>
 </sst>
 </file>
@@ -1139,9 +1298,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6DE93E83-D4E6-9644-A232-80EA76D69371}">
-  <dimension ref="A1:C9"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
@@ -1163,11 +1322,11 @@
       </c>
       <c r="B2" s="4">
         <f>SUMIF(wordcount.txt!B:B,"*elite.bbcelite.com*",wordcount.txt!A:A)</f>
-        <v>225459</v>
+        <v>229655</v>
       </c>
       <c r="C2" s="6">
-        <f>B2/$B$7</f>
-        <v>0.52594266998852279</v>
+        <f>B2/$B$8</f>
+        <v>0.49083432538198324</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1176,53 +1335,66 @@
       </c>
       <c r="B3" s="4">
         <f>SUMIF(wordcount.txt!B:B,"*revs.bbcelite.com*",wordcount.txt!A:A)</f>
-        <v>125771</v>
+        <v>125448</v>
       </c>
       <c r="C3" s="6">
-        <f>B3/$B$7</f>
-        <v>0.29339407851150984</v>
+        <f>B3/$B$8</f>
+        <v>0.26811601946623864</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
-        <v>2</v>
+        <v>295</v>
       </c>
       <c r="B4" s="4">
-        <f>SUMIF(wordcount.txt!B:B,"*aviator.bbcelite.com*",wordcount.txt!A:A)</f>
-        <v>41264</v>
+        <f>SUMIF(wordcount.txt!B:B,"*thesentinel.bbcelite.com*",wordcount.txt!A:A)</f>
+        <v>34649</v>
       </c>
       <c r="C4" s="6">
-        <f>B4/$B$7</f>
-        <v>9.6259179426886513E-2</v>
+        <f>B4/$B$8</f>
+        <v>7.4054205395747266E-2</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B5" s="4">
+        <f>SUMIF(wordcount.txt!B:B,"*aviator.bbcelite.com*",wordcount.txt!A:A)</f>
+        <v>41392</v>
+      </c>
+      <c r="C5" s="6">
+        <f>B5/$B$8</f>
+        <v>8.8465804777649301E-2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B5" s="4">
+      <c r="B6" s="4">
         <f>SUMIF(wordcount.txt!B:B,"*lander.bbcelite.com*",wordcount.txt!A:A)</f>
-        <v>36182</v>
-      </c>
-      <c r="C5" s="6">
-        <f>B5/$B$7</f>
-        <v>8.440407207308083E-2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="B6" s="4"/>
-    </row>
-    <row r="7" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+        <v>36743</v>
+      </c>
+      <c r="C6" s="6">
+        <f>B6/$B$8</f>
+        <v>7.8529644978381538E-2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="B7" s="4"/>
+    </row>
+    <row r="8" spans="1:3" s="3" customFormat="1" x14ac:dyDescent="0.2">
+      <c r="A8" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="B7" s="5">
-        <f>SUM(B2:B5)</f>
-        <v>428676</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="1" t="s">
+      <c r="B8" s="5">
+        <f>SUM(B2:B6)</f>
+        <v>467887</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="1" t="s">
         <v>7</v>
       </c>
     </row>
@@ -1234,10 +1406,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6CB40F6A-245F-024F-9684-E7DD745D31B2}">
-  <dimension ref="A1:B235"/>
+  <dimension ref="A1:B287"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:B236"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B288"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1272,7 +1444,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A4" s="1">
-        <v>5185</v>
+        <v>6003</v>
       </c>
       <c r="B4" t="s">
         <v>222</v>
@@ -1280,7 +1452,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A5" s="1">
-        <v>4163</v>
+        <v>4103</v>
       </c>
       <c r="B5" t="s">
         <v>10</v>
@@ -1296,7 +1468,7 @@
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
-        <v>3402</v>
+        <v>3370</v>
       </c>
       <c r="B7" t="s">
         <v>223</v>
@@ -1304,7 +1476,7 @@
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
-        <v>3201</v>
+        <v>3191</v>
       </c>
       <c r="B8" t="s">
         <v>238</v>
@@ -1344,55 +1516,55 @@
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A13" s="1">
-        <v>2846</v>
+        <v>2862</v>
       </c>
       <c r="B13" t="s">
-        <v>224</v>
+        <v>17</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A14" s="1">
-        <v>2826</v>
+        <v>2846</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>224</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A15" s="1">
-        <v>2783</v>
+        <v>2817</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A16" s="1">
-        <v>2710</v>
+        <v>2783</v>
       </c>
       <c r="B16" t="s">
-        <v>30</v>
+        <v>14</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="1">
-        <v>2707</v>
+        <v>2730</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>30</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="1">
-        <v>2666</v>
+        <v>2709</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="1">
-        <v>2650</v>
+        <v>2638</v>
       </c>
       <c r="B19" t="s">
         <v>18</v>
@@ -1408,10 +1580,10 @@
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="1">
-        <v>2607</v>
+        <v>2582</v>
       </c>
       <c r="B21" t="s">
-        <v>240</v>
+        <v>20</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.2">
@@ -1419,7 +1591,7 @@
         <v>2569</v>
       </c>
       <c r="B22" t="s">
-        <v>20</v>
+        <v>240</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
@@ -1432,330 +1604,330 @@
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="1">
-        <v>2462</v>
+        <v>2508</v>
       </c>
       <c r="B24" t="s">
-        <v>19</v>
+        <v>243</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="1">
-        <v>2401</v>
+        <v>2462</v>
       </c>
       <c r="B25" t="s">
-        <v>241</v>
+        <v>19</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="1">
-        <v>2398</v>
+        <v>2401</v>
       </c>
       <c r="B26" t="s">
-        <v>21</v>
+        <v>241</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="1">
-        <v>2377</v>
+        <v>2398</v>
       </c>
       <c r="B27" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="1">
-        <v>2321</v>
+        <v>2377</v>
       </c>
       <c r="B28" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="1">
-        <v>2314</v>
+        <v>2321</v>
       </c>
       <c r="B29" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="1">
-        <v>2308</v>
+        <v>2314</v>
       </c>
       <c r="B30" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="1">
-        <v>2283</v>
+        <v>2308</v>
       </c>
       <c r="B31" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="1">
-        <v>2221</v>
+        <v>2283</v>
       </c>
       <c r="B32" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="1">
-        <v>2215</v>
+        <v>2221</v>
       </c>
       <c r="B33" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="1">
-        <v>2135</v>
+        <v>2216</v>
       </c>
       <c r="B34" t="s">
-        <v>226</v>
+        <v>28</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
-        <v>2134</v>
+        <v>2176</v>
       </c>
       <c r="B35" t="s">
-        <v>227</v>
+        <v>31</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
-        <v>2133</v>
+        <v>2135</v>
       </c>
       <c r="B36" t="s">
-        <v>31</v>
+        <v>226</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
-        <v>2035</v>
+        <v>2097</v>
       </c>
       <c r="B37" t="s">
-        <v>32</v>
+        <v>227</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A38" s="1">
-        <v>1961</v>
+        <v>2076</v>
       </c>
       <c r="B38" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A39" s="1">
-        <v>1956</v>
+        <v>2035</v>
       </c>
       <c r="B39" t="s">
-        <v>228</v>
+        <v>32</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
-        <v>1922</v>
+        <v>1984</v>
       </c>
       <c r="B40" t="s">
-        <v>33</v>
+        <v>50</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
-        <v>1913</v>
+        <v>1961</v>
       </c>
       <c r="B41" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
-        <v>1887</v>
+        <v>1956</v>
       </c>
       <c r="B42" t="s">
-        <v>36</v>
+        <v>228</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
-        <v>1870</v>
+        <v>1922</v>
       </c>
       <c r="B43" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
-        <v>1857</v>
+        <v>1913</v>
       </c>
       <c r="B44" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
-        <v>1834</v>
+        <v>1887</v>
       </c>
       <c r="B45" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A46" s="1">
-        <v>1829</v>
+        <v>1870</v>
       </c>
       <c r="B46" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A47" s="1">
-        <v>1795</v>
+        <v>1857</v>
       </c>
       <c r="B47" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
-        <v>1794</v>
+        <v>1834</v>
       </c>
       <c r="B48" t="s">
-        <v>34</v>
+        <v>29</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
-        <v>1786</v>
+        <v>1829</v>
       </c>
       <c r="B49" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
-        <v>1758</v>
+        <v>1795</v>
       </c>
       <c r="B50" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
-        <v>1727</v>
+        <v>1794</v>
       </c>
       <c r="B51" t="s">
-        <v>43</v>
+        <v>34</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
-        <v>1716</v>
+        <v>1786</v>
       </c>
       <c r="B52" t="s">
-        <v>229</v>
+        <v>46</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
-        <v>1714</v>
+        <v>1758</v>
       </c>
       <c r="B53" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
-        <v>1690</v>
+        <v>1727</v>
       </c>
       <c r="B54" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
-        <v>1652</v>
+        <v>1714</v>
       </c>
       <c r="B55" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
-        <v>1619</v>
+        <v>1694</v>
       </c>
       <c r="B56" t="s">
-        <v>52</v>
+        <v>229</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
-        <v>1600</v>
+        <v>1690</v>
       </c>
       <c r="B57" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
-        <v>1593</v>
+        <v>1652</v>
       </c>
       <c r="B58" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
-        <v>1587</v>
+        <v>1617</v>
       </c>
       <c r="B59" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A60" s="1">
-        <v>1580</v>
+        <v>1600</v>
       </c>
       <c r="B60" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A61" s="1">
-        <v>1579</v>
+        <v>1593</v>
       </c>
       <c r="B61" t="s">
-        <v>116</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
-        <v>1571</v>
+        <v>1579</v>
       </c>
       <c r="B62" t="s">
-        <v>54</v>
+        <v>116</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
-        <v>1570</v>
+        <v>1571</v>
       </c>
       <c r="B63" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
-        <v>1558</v>
+        <v>1570</v>
       </c>
       <c r="B64" t="s">
-        <v>56</v>
+        <v>51</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.2">
@@ -1768,82 +1940,82 @@
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
-        <v>1513</v>
+        <v>1522</v>
       </c>
       <c r="B66" t="s">
-        <v>57</v>
+        <v>62</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
-        <v>1506</v>
+        <v>1513</v>
       </c>
       <c r="B67" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
-        <v>1471</v>
+        <v>1506</v>
       </c>
       <c r="B68" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A69" s="1">
-        <v>1453</v>
+        <v>1474</v>
       </c>
       <c r="B69" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
-        <v>1450</v>
+        <v>1453</v>
       </c>
       <c r="B70" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
-        <v>1433</v>
+        <v>1450</v>
       </c>
       <c r="B71" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
-        <v>1409</v>
+        <v>1411</v>
       </c>
       <c r="B72" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A73" s="1">
-        <v>1390</v>
+        <v>1409</v>
       </c>
       <c r="B73" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
-        <v>1388</v>
+        <v>1390</v>
       </c>
       <c r="B74" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
-        <v>1354</v>
+        <v>1388</v>
       </c>
       <c r="B75" t="s">
-        <v>64</v>
+        <v>68</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.2">
@@ -1856,10 +2028,10 @@
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
-        <v>1310</v>
+        <v>1332</v>
       </c>
       <c r="B77" t="s">
-        <v>74</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.2">
@@ -1872,50 +2044,50 @@
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
-        <v>1287</v>
+        <v>1288</v>
       </c>
       <c r="B79" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
-        <v>1282</v>
+        <v>1287</v>
       </c>
       <c r="B80" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
-        <v>1271</v>
+        <v>1282</v>
       </c>
       <c r="B81" t="s">
-        <v>242</v>
+        <v>70</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
-        <v>1263</v>
+        <v>1271</v>
       </c>
       <c r="B82" t="s">
-        <v>80</v>
+        <v>242</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
-        <v>1238</v>
+        <v>1263</v>
       </c>
       <c r="B83" t="s">
-        <v>72</v>
+        <v>80</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
-        <v>1221</v>
+        <v>1238</v>
       </c>
       <c r="B84" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.2">
@@ -1928,58 +2100,58 @@
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
-        <v>1136</v>
+        <v>1199</v>
       </c>
       <c r="B86" t="s">
-        <v>230</v>
+        <v>76</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
-        <v>1127</v>
+        <v>1171</v>
       </c>
       <c r="B87" t="s">
-        <v>231</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
-        <v>1125</v>
+        <v>1136</v>
       </c>
       <c r="B88" t="s">
-        <v>79</v>
+        <v>230</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
-        <v>1114</v>
+        <v>1127</v>
       </c>
       <c r="B89" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
-        <v>1104</v>
+        <v>1125</v>
       </c>
       <c r="B90" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
-        <v>1085</v>
+        <v>1114</v>
       </c>
       <c r="B91" t="s">
-        <v>81</v>
+        <v>232</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
-        <v>1083</v>
+        <v>1104</v>
       </c>
       <c r="B92" t="s">
-        <v>73</v>
+        <v>77</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.2">
@@ -1992,10 +2164,10 @@
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
-        <v>1039</v>
+        <v>1071</v>
       </c>
       <c r="B94" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.2">
@@ -2008,10 +2180,10 @@
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
-        <v>1027</v>
+        <v>1028</v>
       </c>
       <c r="B96" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.2">
@@ -2019,7 +2191,7 @@
         <v>1027</v>
       </c>
       <c r="B97" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.2">
@@ -2040,98 +2212,98 @@
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
-        <v>1006</v>
+        <v>1014</v>
       </c>
       <c r="B100" t="s">
-        <v>92</v>
+        <v>113</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
-        <v>950</v>
+        <v>1006</v>
       </c>
       <c r="B101" t="s">
-        <v>86</v>
+        <v>92</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
-        <v>933</v>
+        <v>950</v>
       </c>
       <c r="B102" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
-        <v>928</v>
+        <v>949</v>
       </c>
       <c r="B103" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
-        <v>914</v>
+        <v>928</v>
       </c>
       <c r="B104" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
-        <v>903</v>
+        <v>915</v>
       </c>
       <c r="B105" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A106" s="1">
-        <v>887</v>
+        <v>895</v>
       </c>
       <c r="B106" t="s">
-        <v>234</v>
+        <v>97</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A107" s="1">
-        <v>873</v>
+        <v>869</v>
       </c>
       <c r="B107" t="s">
-        <v>90</v>
+        <v>91</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
-        <v>869</v>
+        <v>865</v>
       </c>
       <c r="B108" t="s">
-        <v>91</v>
+        <v>234</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
-        <v>838</v>
+        <v>865</v>
       </c>
       <c r="B109" t="s">
-        <v>93</v>
+        <v>90</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
-        <v>817</v>
+        <v>838</v>
       </c>
       <c r="B110" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
-        <v>806</v>
+        <v>817</v>
       </c>
       <c r="B111" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.2">
@@ -2139,36 +2311,36 @@
         <v>806</v>
       </c>
       <c r="B112" t="s">
-        <v>95</v>
+        <v>96</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
-        <v>802</v>
+        <v>806</v>
       </c>
       <c r="B113" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
-        <v>771</v>
+        <v>802</v>
       </c>
       <c r="B114" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A115" s="1">
-        <v>746</v>
+        <v>771</v>
       </c>
       <c r="B115" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
-        <v>737</v>
+        <v>769</v>
       </c>
       <c r="B116" t="s">
         <v>101</v>
@@ -2176,50 +2348,50 @@
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
-        <v>734</v>
+        <v>746</v>
       </c>
       <c r="B117" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
-        <v>713</v>
+        <v>734</v>
       </c>
       <c r="B118" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="119" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
-        <v>667</v>
+        <v>713</v>
       </c>
       <c r="B119" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="120" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
-        <v>590</v>
+        <v>663</v>
       </c>
       <c r="B120" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
     </row>
     <row r="121" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
-        <v>559</v>
+        <v>584</v>
       </c>
       <c r="B121" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="122" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
-        <v>558</v>
+        <v>559</v>
       </c>
       <c r="B122" t="s">
-        <v>235</v>
+        <v>106</v>
       </c>
     </row>
     <row r="123" spans="1:2" x14ac:dyDescent="0.2">
@@ -2232,26 +2404,26 @@
     </row>
     <row r="124" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
-        <v>537</v>
+        <v>552</v>
       </c>
       <c r="B124" t="s">
-        <v>108</v>
+        <v>235</v>
       </c>
     </row>
     <row r="125" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
-        <v>487</v>
+        <v>537</v>
       </c>
       <c r="B125" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="126" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
-        <v>486</v>
+        <v>487</v>
       </c>
       <c r="B126" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
     </row>
     <row r="127" spans="1:2" x14ac:dyDescent="0.2">
@@ -2259,191 +2431,191 @@
         <v>486</v>
       </c>
       <c r="B127" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="128" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A128" s="1">
-        <v>476</v>
+        <v>486</v>
       </c>
       <c r="B128" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="129" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
-        <v>353</v>
+        <v>476</v>
       </c>
       <c r="B129" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="130" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
-        <v>339</v>
+        <v>353</v>
       </c>
       <c r="B130" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="131" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
-        <v>273</v>
+        <v>339</v>
       </c>
       <c r="B131" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
     <row r="132" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
-        <v>7326</v>
+        <v>273</v>
       </c>
       <c r="B132" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
     </row>
     <row r="133" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
-        <v>5383</v>
+        <v>7325</v>
       </c>
       <c r="B133" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
     </row>
     <row r="134" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
-        <v>5182</v>
+        <v>5383</v>
       </c>
       <c r="B134" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
     </row>
     <row r="135" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
-        <v>4858</v>
+        <v>5182</v>
       </c>
       <c r="B135" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
     </row>
     <row r="136" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A136" s="1">
-        <v>4837</v>
+        <v>4854</v>
       </c>
       <c r="B136" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
     </row>
     <row r="137" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
-        <v>4702</v>
+        <v>4837</v>
       </c>
       <c r="B137" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="138" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
-        <v>4682</v>
+        <v>4702</v>
       </c>
       <c r="B138" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
     </row>
     <row r="139" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
-        <v>4004</v>
+        <v>4659</v>
       </c>
       <c r="B139" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="140" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
-        <v>3775</v>
+        <v>4004</v>
       </c>
       <c r="B140" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
     </row>
     <row r="141" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
-        <v>3688</v>
+        <v>3775</v>
       </c>
       <c r="B141" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
     </row>
     <row r="142" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
-        <v>3646</v>
+        <v>3684</v>
       </c>
       <c r="B142" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
     </row>
     <row r="143" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
-        <v>3640</v>
+        <v>3646</v>
       </c>
       <c r="B143" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
     </row>
     <row r="144" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
-        <v>3293</v>
+        <v>3627</v>
       </c>
       <c r="B144" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
     </row>
     <row r="145" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
-        <v>3267</v>
+        <v>3293</v>
       </c>
       <c r="B145" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
     </row>
     <row r="146" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
-        <v>3208</v>
+        <v>3178</v>
       </c>
       <c r="B146" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
     </row>
     <row r="147" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
-        <v>3178</v>
+        <v>3168</v>
       </c>
       <c r="B147" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
     </row>
     <row r="148" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
-        <v>3156</v>
+        <v>3109</v>
       </c>
       <c r="B148" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
     </row>
     <row r="149" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
-        <v>3074</v>
+        <v>3057</v>
       </c>
       <c r="B149" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
     </row>
     <row r="150" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
-        <v>3007</v>
+        <v>2975</v>
       </c>
       <c r="B150" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
     </row>
     <row r="151" spans="1:2" x14ac:dyDescent="0.2">
@@ -2456,10 +2628,10 @@
     </row>
     <row r="152" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
-        <v>2857</v>
+        <v>2908</v>
       </c>
       <c r="B152" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
     </row>
     <row r="153" spans="1:2" x14ac:dyDescent="0.2">
@@ -2472,58 +2644,58 @@
     </row>
     <row r="154" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
-        <v>2550</v>
+        <v>2758</v>
       </c>
       <c r="B154" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
     </row>
     <row r="155" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
-        <v>2524</v>
+        <v>2550</v>
       </c>
       <c r="B155" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
     </row>
     <row r="156" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
-        <v>2489</v>
+        <v>2524</v>
       </c>
       <c r="B156" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
     </row>
     <row r="157" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
-        <v>2188</v>
+        <v>2489</v>
       </c>
       <c r="B157" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
     </row>
     <row r="158" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A158" s="1">
-        <v>2080</v>
+        <v>2280</v>
       </c>
       <c r="B158" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
     </row>
     <row r="159" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A159" s="1">
-        <v>1966</v>
+        <v>2188</v>
       </c>
       <c r="B159" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
     </row>
     <row r="160" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
-        <v>1890</v>
+        <v>2080</v>
       </c>
       <c r="B160" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
     </row>
     <row r="161" spans="1:2" x14ac:dyDescent="0.2">
@@ -2536,183 +2708,183 @@
     </row>
     <row r="162" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
-        <v>1675</v>
+        <v>1848</v>
       </c>
       <c r="B162" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
     </row>
     <row r="163" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
-        <v>1585</v>
+        <v>1675</v>
       </c>
       <c r="B163" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
     </row>
     <row r="164" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
-        <v>1582</v>
+        <v>1629</v>
       </c>
       <c r="B164" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
     </row>
     <row r="165" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
-        <v>1427</v>
+        <v>1582</v>
       </c>
       <c r="B165" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
     </row>
     <row r="166" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
-        <v>1405</v>
+        <v>1427</v>
       </c>
       <c r="B166" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="167" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
-        <v>1320</v>
+        <v>1405</v>
       </c>
       <c r="B167" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
     </row>
     <row r="168" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A168" s="1">
-        <v>1283</v>
+        <v>1320</v>
       </c>
       <c r="B168" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
-        <v>1148</v>
+        <v>1283</v>
       </c>
       <c r="B169" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
     </row>
     <row r="170" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
-        <v>1122</v>
+        <v>1148</v>
       </c>
       <c r="B170" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
     </row>
     <row r="171" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
-        <v>1065</v>
+        <v>1122</v>
       </c>
       <c r="B171" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
     </row>
     <row r="172" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
-        <v>1040</v>
+        <v>1065</v>
       </c>
       <c r="B172" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
     </row>
     <row r="173" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
-        <v>1010</v>
+        <v>1040</v>
       </c>
       <c r="B173" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
     </row>
     <row r="174" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
-        <v>1004</v>
+        <v>1010</v>
       </c>
       <c r="B174" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
     </row>
     <row r="175" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
-        <v>973</v>
+        <v>1004</v>
       </c>
       <c r="B175" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
     </row>
     <row r="176" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
-        <v>888</v>
+        <v>973</v>
       </c>
       <c r="B176" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
     </row>
     <row r="177" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
-        <v>842</v>
+        <v>888</v>
       </c>
       <c r="B177" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
     </row>
     <row r="178" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
-        <v>735</v>
+        <v>842</v>
       </c>
       <c r="B178" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
     </row>
     <row r="179" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A179" s="1">
-        <v>717</v>
+        <v>735</v>
       </c>
       <c r="B179" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
     </row>
     <row r="180" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
-        <v>562</v>
+        <v>717</v>
       </c>
       <c r="B180" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
     </row>
     <row r="181" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
-        <v>285</v>
+        <v>562</v>
       </c>
       <c r="B181" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
     </row>
     <row r="182" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
-        <v>3627</v>
+        <v>285</v>
       </c>
       <c r="B182" t="s">
-        <v>168</v>
+        <v>167</v>
       </c>
     </row>
     <row r="183" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
-        <v>2508</v>
+        <v>3627</v>
       </c>
       <c r="B183" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
     </row>
     <row r="184" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
-        <v>2367</v>
+        <v>2536</v>
       </c>
       <c r="B184" t="s">
         <v>170</v>
@@ -2720,114 +2892,114 @@
     </row>
     <row r="185" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
-        <v>2117</v>
+        <v>2508</v>
       </c>
       <c r="B185" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
     </row>
     <row r="186" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
-        <v>2027</v>
+        <v>2117</v>
       </c>
       <c r="B186" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
     </row>
     <row r="187" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
-        <v>1587</v>
+        <v>2027</v>
       </c>
       <c r="B187" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
     </row>
     <row r="188" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
-        <v>1532</v>
+        <v>1548</v>
       </c>
       <c r="B188" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="189" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
-        <v>1369</v>
+        <v>1532</v>
       </c>
       <c r="B189" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
     </row>
     <row r="190" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
-        <v>1368</v>
+        <v>1369</v>
       </c>
       <c r="B190" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
     </row>
     <row r="191" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
-        <v>1349</v>
+        <v>1368</v>
       </c>
       <c r="B191" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
     </row>
     <row r="192" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
-        <v>1336</v>
+        <v>1349</v>
       </c>
       <c r="B192" t="s">
-        <v>178</v>
+        <v>177</v>
       </c>
     </row>
     <row r="193" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
-        <v>1312</v>
+        <v>1336</v>
       </c>
       <c r="B193" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
     </row>
     <row r="194" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
-        <v>1299</v>
+        <v>1312</v>
       </c>
       <c r="B194" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
     </row>
     <row r="195" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
-        <v>1267</v>
+        <v>1299</v>
       </c>
       <c r="B195" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
     </row>
     <row r="196" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
-        <v>1260</v>
+        <v>1267</v>
       </c>
       <c r="B196" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
     </row>
     <row r="197" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
-        <v>1258</v>
+        <v>1260</v>
       </c>
       <c r="B197" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
     </row>
     <row r="198" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
-        <v>1147</v>
+        <v>1258</v>
       </c>
       <c r="B198" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
     </row>
     <row r="199" spans="1:2" x14ac:dyDescent="0.2">
@@ -2835,294 +3007,710 @@
         <v>1147</v>
       </c>
       <c r="B199" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
     </row>
     <row r="200" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
-        <v>1145</v>
+        <v>1147</v>
       </c>
       <c r="B200" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
     </row>
     <row r="201" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
-        <v>1139</v>
+        <v>1145</v>
       </c>
       <c r="B201" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
     </row>
     <row r="202" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
-        <v>1074</v>
+        <v>1137</v>
       </c>
       <c r="B202" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
     </row>
     <row r="203" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
-        <v>1025</v>
+        <v>1074</v>
       </c>
       <c r="B203" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
     </row>
     <row r="204" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
-        <v>910</v>
+        <v>1025</v>
       </c>
       <c r="B204" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
     </row>
     <row r="205" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
-        <v>892</v>
+        <v>910</v>
       </c>
       <c r="B205" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
     </row>
     <row r="206" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
-        <v>887</v>
+        <v>892</v>
       </c>
       <c r="B206" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
     </row>
     <row r="207" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
-        <v>749</v>
+        <v>887</v>
       </c>
       <c r="B207" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
     </row>
     <row r="208" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
-        <v>676</v>
+        <v>749</v>
       </c>
       <c r="B208" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
     </row>
     <row r="209" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
-        <v>673</v>
+        <v>676</v>
       </c>
       <c r="B209" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
     </row>
     <row r="210" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
-        <v>641</v>
+        <v>673</v>
       </c>
       <c r="B210" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
     </row>
     <row r="211" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
-        <v>613</v>
+        <v>641</v>
       </c>
       <c r="B211" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
     </row>
     <row r="212" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
-        <v>593</v>
+        <v>613</v>
       </c>
       <c r="B212" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
     </row>
     <row r="213" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
-        <v>370</v>
+        <v>593</v>
       </c>
       <c r="B213" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
     </row>
     <row r="214" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
-        <v>3252</v>
+        <v>370</v>
       </c>
       <c r="B214" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
     </row>
     <row r="215" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
-        <v>3028</v>
+        <v>4347</v>
       </c>
       <c r="B215" t="s">
-        <v>201</v>
+        <v>244</v>
       </c>
     </row>
     <row r="216" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
-        <v>3015</v>
+        <v>3269</v>
       </c>
       <c r="B216" t="s">
-        <v>202</v>
+        <v>245</v>
       </c>
     </row>
     <row r="217" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
-        <v>2939</v>
+        <v>2225</v>
       </c>
       <c r="B217" t="s">
-        <v>203</v>
+        <v>246</v>
       </c>
     </row>
     <row r="218" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
-        <v>2793</v>
+        <v>1951</v>
       </c>
       <c r="B218" t="s">
-        <v>204</v>
+        <v>247</v>
       </c>
     </row>
     <row r="219" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
-        <v>2613</v>
+        <v>1702</v>
       </c>
       <c r="B219" t="s">
-        <v>205</v>
+        <v>248</v>
       </c>
     </row>
     <row r="220" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
-        <v>2602</v>
+        <v>1505</v>
       </c>
       <c r="B220" t="s">
-        <v>206</v>
+        <v>249</v>
       </c>
     </row>
     <row r="221" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
-        <v>2170</v>
+        <v>1492</v>
       </c>
       <c r="B221" t="s">
-        <v>207</v>
+        <v>250</v>
       </c>
     </row>
     <row r="222" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
-        <v>1924</v>
+        <v>1474</v>
       </c>
       <c r="B222" t="s">
-        <v>208</v>
+        <v>251</v>
       </c>
     </row>
     <row r="223" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
-        <v>1517</v>
+        <v>1270</v>
       </c>
       <c r="B223" t="s">
-        <v>209</v>
+        <v>252</v>
       </c>
     </row>
     <row r="224" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
-        <v>1424</v>
+        <v>1253</v>
       </c>
       <c r="B224" t="s">
-        <v>210</v>
+        <v>253</v>
       </c>
     </row>
     <row r="225" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A225" s="1">
-        <v>1384</v>
+        <v>1223</v>
       </c>
       <c r="B225" t="s">
-        <v>211</v>
+        <v>254</v>
       </c>
     </row>
     <row r="226" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
-        <v>1225</v>
+        <v>1188</v>
       </c>
       <c r="B226" t="s">
-        <v>212</v>
+        <v>255</v>
       </c>
     </row>
     <row r="227" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
-        <v>1037</v>
+        <v>1166</v>
       </c>
       <c r="B227" t="s">
-        <v>213</v>
+        <v>256</v>
       </c>
     </row>
     <row r="228" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
-        <v>874</v>
+        <v>1097</v>
       </c>
       <c r="B228" t="s">
-        <v>214</v>
+        <v>257</v>
       </c>
     </row>
     <row r="229" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
-        <v>851</v>
+        <v>1069</v>
       </c>
       <c r="B229" t="s">
-        <v>215</v>
+        <v>258</v>
       </c>
     </row>
     <row r="230" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
-        <v>799</v>
+        <v>1015</v>
       </c>
       <c r="B230" t="s">
-        <v>216</v>
+        <v>259</v>
       </c>
     </row>
     <row r="231" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
-        <v>667</v>
+        <v>943</v>
       </c>
       <c r="B231" t="s">
-        <v>217</v>
+        <v>260</v>
       </c>
     </row>
     <row r="232" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
-        <v>665</v>
+        <v>861</v>
       </c>
       <c r="B232" t="s">
-        <v>218</v>
+        <v>261</v>
       </c>
     </row>
     <row r="233" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
-        <v>483</v>
+        <v>664</v>
       </c>
       <c r="B233" t="s">
-        <v>219</v>
+        <v>262</v>
       </c>
     </row>
     <row r="234" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
-        <v>468</v>
+        <v>626</v>
       </c>
       <c r="B234" t="s">
-        <v>220</v>
+        <v>263</v>
       </c>
     </row>
     <row r="235" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
+        <v>575</v>
+      </c>
+      <c r="B235" t="s">
+        <v>264</v>
+      </c>
+    </row>
+    <row r="236" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A236" s="1">
+        <v>520</v>
+      </c>
+      <c r="B236" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="237" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A237" s="1">
+        <v>283</v>
+      </c>
+      <c r="B237" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="238" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A238" s="1">
+        <v>271</v>
+      </c>
+      <c r="B238" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="239" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A239" s="1">
+        <v>186</v>
+      </c>
+      <c r="B239" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="240" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A240" s="1">
+        <v>184</v>
+      </c>
+      <c r="B240" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="241" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A241" s="1">
+        <v>180</v>
+      </c>
+      <c r="B241" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="242" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A242" s="1">
+        <v>129</v>
+      </c>
+      <c r="B242" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="243" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A243" s="1">
+        <v>115</v>
+      </c>
+      <c r="B243" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="244" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A244" s="1">
+        <v>105</v>
+      </c>
+      <c r="B244" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="245" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A245" s="1">
+        <v>95</v>
+      </c>
+      <c r="B245" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="246" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A246" s="1">
+        <v>91</v>
+      </c>
+      <c r="B246" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="247" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A247" s="1">
+        <v>90</v>
+      </c>
+      <c r="B247" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="248" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A248" s="1">
+        <v>89</v>
+      </c>
+      <c r="B248" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="249" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A249" s="1">
+        <v>87</v>
+      </c>
+      <c r="B249" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="250" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A250" s="1">
+        <v>86</v>
+      </c>
+      <c r="B250" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="251" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A251" s="1">
+        <v>86</v>
+      </c>
+      <c r="B251" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="252" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A252" s="1">
+        <v>85</v>
+      </c>
+      <c r="B252" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="253" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A253" s="1">
+        <v>84</v>
+      </c>
+      <c r="B253" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="254" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A254" s="1">
+        <v>83</v>
+      </c>
+      <c r="B254" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="255" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A255" s="1">
+        <v>83</v>
+      </c>
+      <c r="B255" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="256" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A256" s="1">
+        <v>82</v>
+      </c>
+      <c r="B256" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="257" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A257" s="1">
+        <v>82</v>
+      </c>
+      <c r="B257" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="258" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A258" s="1">
+        <v>81</v>
+      </c>
+      <c r="B258" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="259" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A259" s="1">
+        <v>81</v>
+      </c>
+      <c r="B259" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="260" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A260" s="1">
+        <v>81</v>
+      </c>
+      <c r="B260" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="261" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A261" s="1">
+        <v>81</v>
+      </c>
+      <c r="B261" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="262" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A262" s="1">
+        <v>81</v>
+      </c>
+      <c r="B262" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="263" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A263" s="1">
+        <v>78</v>
+      </c>
+      <c r="B263" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="264" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A264" s="1">
+        <v>78</v>
+      </c>
+      <c r="B264" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="265" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A265" s="1">
+        <v>77</v>
+      </c>
+      <c r="B265" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="266" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A266" s="1">
+        <v>3234</v>
+      </c>
+      <c r="B266" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="267" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A267" s="1">
+        <v>3028</v>
+      </c>
+      <c r="B267" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="268" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A268" s="1">
+        <v>3015</v>
+      </c>
+      <c r="B268" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="269" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A269" s="1">
+        <v>2939</v>
+      </c>
+      <c r="B269" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="270" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A270" s="1">
+        <v>2845</v>
+      </c>
+      <c r="B270" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="271" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A271" s="1">
+        <v>2793</v>
+      </c>
+      <c r="B271" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="272" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A272" s="1">
+        <v>2606</v>
+      </c>
+      <c r="B272" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="273" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A273" s="1">
+        <v>2170</v>
+      </c>
+      <c r="B273" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="274" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A274" s="1">
+        <v>1924</v>
+      </c>
+      <c r="B274" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="275" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A275" s="1">
+        <v>1517</v>
+      </c>
+      <c r="B275" t="s">
+        <v>209</v>
+      </c>
+    </row>
+    <row r="276" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A276" s="1">
+        <v>1490</v>
+      </c>
+      <c r="B276" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="277" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A277" s="1">
+        <v>1417</v>
+      </c>
+      <c r="B277" t="s">
+        <v>210</v>
+      </c>
+    </row>
+    <row r="278" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A278" s="1">
+        <v>1385</v>
+      </c>
+      <c r="B278" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="279" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A279" s="1">
+        <v>1024</v>
+      </c>
+      <c r="B279" t="s">
+        <v>213</v>
+      </c>
+    </row>
+    <row r="280" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A280" s="1">
+        <v>874</v>
+      </c>
+      <c r="B280" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="281" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A281" s="1">
+        <v>851</v>
+      </c>
+      <c r="B281" t="s">
+        <v>215</v>
+      </c>
+    </row>
+    <row r="282" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A282" s="1">
+        <v>799</v>
+      </c>
+      <c r="B282" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="283" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A283" s="1">
+        <v>764</v>
+      </c>
+      <c r="B283" t="s">
+        <v>217</v>
+      </c>
+    </row>
+    <row r="284" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A284" s="1">
+        <v>665</v>
+      </c>
+      <c r="B284" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="285" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A285" s="1">
+        <v>483</v>
+      </c>
+      <c r="B285" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="286" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A286" s="1">
+        <v>468</v>
+      </c>
+      <c r="B286" t="s">
+        <v>220</v>
+      </c>
+    </row>
+    <row r="287" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A287" s="1">
         <v>452</v>
       </c>
-      <c r="B235" t="s">
+      <c r="B287" t="s">
         <v>221</v>
       </c>
     </row>

</xml_diff>